<commit_message>
add phoneNumber format control
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1103,9 +1103,102 @@
         <v>John</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Tue Feb 22 2022</v>
+      </c>
+      <c r="B21" t="str">
+        <v>17:14:42 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C21" t="str">
+        <v>0022892942601</v>
+      </c>
+      <c r="D21" t="str">
+        <v>User</v>
+      </c>
+      <c r="E21" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F21" t="str">
+        <v>request</v>
+      </c>
+      <c r="G21" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H21" t="str">
+        <v>0022892942601 request to receive otp</v>
+      </c>
+      <c r="K21" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Tue Feb 22 2022</v>
+      </c>
+      <c r="B22" t="str">
+        <v>17:18:25 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D22" t="str">
+        <v>User</v>
+      </c>
+      <c r="E22" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F22" t="str">
+        <v>login</v>
+      </c>
+      <c r="G22" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H22" t="str">
+        <v>invalid email  login</v>
+      </c>
+      <c r="K22" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="N22" t="str">
+        <v>invalid email</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Tue Feb 22 2022</v>
+      </c>
+      <c r="B23" t="str">
+        <v>17:20:47 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>User</v>
+      </c>
+      <c r="E23" t="str">
+        <v>/api/user/:id</v>
+      </c>
+      <c r="F23" t="str">
+        <v>read</v>
+      </c>
+      <c r="G23" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H23" t="str">
+        <v>Doe  John  read user 1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="str">
+        <v>1</v>
+      </c>
+      <c r="L23" t="str">
+        <v>Doe</v>
+      </c>
+      <c r="M23" t="str">
+        <v>John</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>